<commit_message>
Minor updates to log statements and global setup.
</commit_message>
<xml_diff>
--- a/Documentation/Motorola Stability Tests.xlsx
+++ b/Documentation/Motorola Stability Tests.xlsx
@@ -5328,8 +5328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5605,7 +5605,7 @@
         <v>158</v>
       </c>
       <c r="C22" s="22">
-        <v>1.7013888888888892E-3</v>
+        <v>4.0972222222222226E-3</v>
       </c>
       <c r="D22" s="2">
         <v>1.29</v>
@@ -5619,7 +5619,7 @@
         <v>159</v>
       </c>
       <c r="C23" s="22">
-        <v>7.8703703703703705E-4</v>
+        <v>3.9351851851851857E-3</v>
       </c>
       <c r="D23" s="2">
         <v>1.29</v>
@@ -5633,7 +5633,7 @@
         <v>160</v>
       </c>
       <c r="C24" s="22">
-        <v>1.9791666666666668E-3</v>
+        <v>4.2476851851851851E-3</v>
       </c>
       <c r="D24" s="2">
         <v>1.29</v>
@@ -5647,7 +5647,7 @@
         <v>161</v>
       </c>
       <c r="C25" s="22">
-        <v>1.0300925925925926E-3</v>
+        <v>3.2175925925925926E-3</v>
       </c>
       <c r="D25" s="2">
         <v>1.29</v>
@@ -5661,7 +5661,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="22">
-        <v>9.4907407407407408E-4</v>
+        <v>3.8425925925925923E-3</v>
       </c>
       <c r="D26" s="2">
         <v>1.29</v>
@@ -5675,7 +5675,7 @@
         <v>163</v>
       </c>
       <c r="C27" s="22">
-        <v>1.4814814814814814E-3</v>
+        <v>4.5833333333333334E-3</v>
       </c>
       <c r="D27" s="2">
         <v>1.29</v>
@@ -5689,7 +5689,7 @@
         <v>164</v>
       </c>
       <c r="C28" s="22">
-        <v>1.4583333333333334E-3</v>
+        <v>3.7847222222222223E-3</v>
       </c>
       <c r="D28" s="2">
         <v>1.29</v>
@@ -5704,7 +5704,7 @@
         <v>165</v>
       </c>
       <c r="C29" s="22">
-        <v>1.2152777777777778E-3</v>
+        <v>3.9236111111111112E-3</v>
       </c>
       <c r="D29" s="2">
         <v>1.29</v>
@@ -5719,7 +5719,7 @@
         <v>166</v>
       </c>
       <c r="C30" s="22">
-        <v>1.2384259259259258E-3</v>
+        <v>3.7615740740740739E-3</v>
       </c>
       <c r="D30" s="2">
         <v>1.29</v>
@@ -5734,7 +5734,7 @@
         <v>167</v>
       </c>
       <c r="C31" s="22">
-        <v>2.5115740740740741E-3</v>
+        <v>3.5069444444444445E-3</v>
       </c>
       <c r="D31" s="2">
         <v>1.29</v>
@@ -5749,7 +5749,7 @@
         <v>168</v>
       </c>
       <c r="C32" s="22">
-        <v>1.25E-3</v>
+        <v>3.8310185185185183E-3</v>
       </c>
       <c r="D32" s="2">
         <v>1.29</v>
@@ -5794,7 +5794,7 @@
         <v>173</v>
       </c>
       <c r="C35" s="22">
-        <v>6.4814814814814813E-3</v>
+        <v>6.9212962962962969E-3</v>
       </c>
       <c r="D35" s="2">
         <v>1.29</v>
@@ -5804,7 +5804,7 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C36" s="23">
         <f>SUM(C22:C35)</f>
-        <v>2.2083333333333333E-2</v>
+        <v>4.9652777777777782E-2</v>
       </c>
       <c r="D36" s="2"/>
       <c r="G36" s="23"/>

</xml_diff>